<commit_message>
missing to fix only the and, maybe improve or
</commit_message>
<xml_diff>
--- a/Gates/Figures/Centered logic_gates_results.xlsx
+++ b/Gates/Figures/Centered logic_gates_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noelfpb/Documents/Research/Scripts/Gates/Figures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noelp\Documents\Kanazawa\Scripts_Kanazawa\Gates\Figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77D2393-D6CE-F64B-84B8-BA9DC716F8D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5ADEEE4-E2C0-4903-A149-6CED9E536396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" xr2:uid="{BB5C9B73-F402-EE4B-B977-48B807FD5169}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BB5C9B73-F402-EE4B-B977-48B807FD5169}"/>
   </bookViews>
   <sheets>
     <sheet name="NORMALIZED" sheetId="1" r:id="rId1"/>
@@ -458,13 +458,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA15B86-EB8F-3842-AF8A-B1DE65170201}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="136" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -478,7 +478,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -492,7 +492,7 @@
         <v>0.33950617283950613</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -506,7 +506,7 @@
         <v>0.23662551440329216</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -521,7 +521,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -535,7 +535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -546,10 +546,10 @@
         <v>0.01</v>
       </c>
       <c r="D6">
-        <v>0.4152542372881356</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.11294173829990449</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -560,10 +560,10 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D7">
-        <v>0.81144067796610175</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.74689589302769821</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -574,11 +574,11 @@
         <v>0.01</v>
       </c>
       <c r="D8">
-        <v>0.97881355932203395</v>
+        <v>0.96991404011461335</v>
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -592,7 +592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -606,7 +606,7 @@
         <v>0.24458204334365327</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -620,7 +620,7 @@
         <v>0.95665634674922595</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -635,7 +635,7 @@
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -649,7 +649,7 @@
         <v>9.9071207430340563E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -660,10 +660,10 @@
         <v>0.01</v>
       </c>
       <c r="D14">
-        <v>0.95801526717557239</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -674,10 +674,10 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.98990228013029324</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -688,11 +688,11 @@
         <v>0.01</v>
       </c>
       <c r="D16">
-        <v>0.95038167938931306</v>
+        <v>0.94429967426710104</v>
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -703,10 +703,10 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D17">
-        <v>0.40839694656488551</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.21889250814332251</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -720,7 +720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -731,10 +731,10 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D19">
-        <v>0.44622425629290619</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.2259156050955414</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -745,11 +745,11 @@
         <v>0.01</v>
       </c>
       <c r="D20">
-        <v>0.30892448512585813</v>
+        <v>0.24860668789808918</v>
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -760,10 +760,10 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D21">
-        <v>0.3386727688787185</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.23686305732484075</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -777,7 +777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -791,7 +791,7 @@
         <v>0.26121372031662271</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -806,7 +806,7 @@
       </c>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -829,16 +829,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E10E3C36-A08C-614C-AF0A-A852E4553B8F}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:E13"/>
+    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -855,7 +855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -873,7 +873,7 @@
         <v>0.33950617283950613</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -891,7 +891,7 @@
         <v>0.23662551440329216</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -909,7 +909,7 @@
         <v>0.23662551440329216</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -927,7 +927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -938,14 +938,14 @@
         <v>0.01</v>
       </c>
       <c r="D6">
-        <v>1.96</v>
+        <v>0.47299999999999998</v>
       </c>
       <c r="E6">
         <f>D6/MAX(D$6:D$9)</f>
-        <v>0.4152542372881356</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.11294173829990449</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -956,14 +956,14 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D7">
-        <v>3.83</v>
+        <v>3.1280000000000001</v>
       </c>
       <c r="E7">
         <f t="shared" ref="E7:E9" si="0">D7/MAX(D$6:D$9)</f>
-        <v>0.81144067796610175</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.74689589302769821</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -974,14 +974,14 @@
         <v>0.01</v>
       </c>
       <c r="D8">
-        <v>4.62</v>
+        <v>4.0620000000000003</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0.97881355932203395</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.96991404011461335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -992,14 +992,14 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D9">
-        <v>4.72</v>
+        <v>4.1879999999999997</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>0.24458204334365327</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>0.95665634674922595</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>9.9071207430340563E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1082,14 +1082,14 @@
         <v>0.01</v>
       </c>
       <c r="D14">
-        <v>2.5099999999999998</v>
+        <v>3.07</v>
       </c>
       <c r="E14">
         <f>D14/MAX(D$14:D$17)</f>
-        <v>0.95801526717557239</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1100,14 +1100,14 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D15">
-        <v>2.62</v>
+        <v>3.0390000000000001</v>
       </c>
       <c r="E15">
         <f t="shared" ref="E15:E17" si="2">D15/MAX(D$14:D$17)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.98990228013029324</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1118,14 +1118,14 @@
         <v>0.01</v>
       </c>
       <c r="D16">
-        <v>2.4900000000000002</v>
+        <v>2.899</v>
       </c>
       <c r="E16">
         <f t="shared" si="2"/>
-        <v>0.95038167938931306</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.94429967426710104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1136,14 +1136,14 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D17">
-        <v>1.07</v>
+        <v>0.67200000000000004</v>
       </c>
       <c r="E17">
         <f t="shared" si="2"/>
-        <v>0.40839694656488551</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.21889250814332251</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1154,14 +1154,14 @@
         <v>0.01</v>
       </c>
       <c r="D18">
-        <v>4.37</v>
+        <v>5.024</v>
       </c>
       <c r="E18">
         <f>D18/MAX(D$18:D$21)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1172,14 +1172,14 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D19">
-        <v>1.95</v>
+        <v>1.135</v>
       </c>
       <c r="E19">
         <f t="shared" ref="E19:E21" si="3">D19/MAX(D$18:D$21)</f>
-        <v>0.44622425629290619</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.2259156050955414</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1190,14 +1190,14 @@
         <v>0.01</v>
       </c>
       <c r="D20">
-        <v>1.35</v>
+        <v>1.2490000000000001</v>
       </c>
       <c r="E20">
         <f t="shared" si="3"/>
-        <v>0.30892448512585813</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.24860668789808918</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1208,14 +1208,14 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D21">
-        <v>1.48</v>
+        <v>1.19</v>
       </c>
       <c r="E21">
         <f t="shared" si="3"/>
-        <v>0.3386727688787185</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.23686305732484075</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>0.26121372031662271</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>0.31662269129287596</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>9</v>
       </c>

</xml_diff>